<commit_message>
Revert "change pagina corporativa"
This reverts commit 16ea66bb455805712a5ad15958004c82952b2986.
</commit_message>
<xml_diff>
--- a/Fichas Tecnicas apps/Ficha de aplicacion - Páginas corporativas.xlsx
+++ b/Fichas Tecnicas apps/Ficha de aplicacion - Páginas corporativas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="62">
   <si>
     <t>Nombre de la aplicación:</t>
   </si>
@@ -202,9 +202,6 @@
   </si>
   <si>
     <t>WEBLOGIC 12</t>
-  </si>
-  <si>
-    <t>Media</t>
   </si>
 </sst>
 </file>
@@ -408,12 +405,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="4" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -424,6 +415,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -911,8 +908,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C25" sqref="C25:D25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -937,69 +934,67 @@
       <c r="A6" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
-      <c r="G6" s="13"/>
-      <c r="H6" s="13"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
+      <c r="G6" s="11"/>
+      <c r="H6" s="11"/>
     </row>
     <row r="7" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="13" t="s">
+      <c r="B7" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="C7" s="13"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="13"/>
-      <c r="F7" s="13"/>
-      <c r="G7" s="13"/>
-      <c r="H7" s="13"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
+      <c r="G7" s="11"/>
+      <c r="H7" s="11"/>
     </row>
     <row r="8" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="B8" s="14"/>
-      <c r="C8" s="14"/>
-      <c r="D8" s="14"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="14"/>
-      <c r="G8" s="14"/>
-      <c r="H8" s="14"/>
+      <c r="B8" s="12"/>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12"/>
+      <c r="E8" s="12"/>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="12"/>
     </row>
     <row r="9" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="B9" s="13" t="s">
+      <c r="B9" s="11" t="s">
         <v>45</v>
       </c>
-      <c r="C9" s="13"/>
-      <c r="D9" s="13"/>
-      <c r="E9" s="13"/>
-      <c r="F9" s="13"/>
-      <c r="G9" s="13"/>
-      <c r="H9" s="13"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+      <c r="G9" s="11"/>
+      <c r="H9" s="11"/>
     </row>
     <row r="10" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B10" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C10" s="13"/>
-      <c r="D10" s="13"/>
-      <c r="E10" s="13"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="13"/>
-      <c r="H10" s="13"/>
+      <c r="B10" s="11"/>
+      <c r="C10" s="11"/>
+      <c r="D10" s="11"/>
+      <c r="E10" s="11"/>
+      <c r="F10" s="11"/>
+      <c r="G10" s="11"/>
+      <c r="H10" s="11"/>
     </row>
     <row r="11" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
@@ -1019,115 +1014,115 @@
       <c r="A12" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B12" s="13"/>
-      <c r="C12" s="13"/>
-      <c r="D12" s="13"/>
-      <c r="E12" s="13"/>
-      <c r="F12" s="13"/>
-      <c r="G12" s="13"/>
-      <c r="H12" s="13"/>
+      <c r="B12" s="11"/>
+      <c r="C12" s="11"/>
+      <c r="D12" s="11"/>
+      <c r="E12" s="11"/>
+      <c r="F12" s="11"/>
+      <c r="G12" s="11"/>
+      <c r="H12" s="11"/>
     </row>
     <row r="13" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="B13" s="13"/>
-      <c r="C13" s="13"/>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13"/>
-      <c r="F13" s="13"/>
-      <c r="G13" s="13"/>
-      <c r="H13" s="13"/>
+      <c r="B13" s="11"/>
+      <c r="C13" s="11"/>
+      <c r="D13" s="11"/>
+      <c r="E13" s="11"/>
+      <c r="F13" s="11"/>
+      <c r="G13" s="11"/>
+      <c r="H13" s="11"/>
     </row>
     <row r="14" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="13"/>
-      <c r="C14" s="13"/>
-      <c r="D14" s="13"/>
-      <c r="E14" s="13"/>
-      <c r="F14" s="13"/>
-      <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
+      <c r="B14" s="11"/>
+      <c r="C14" s="11"/>
+      <c r="D14" s="11"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="11"/>
+      <c r="G14" s="11"/>
+      <c r="H14" s="11"/>
     </row>
     <row r="15" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="B15" s="13" t="s">
+      <c r="B15" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="C15" s="13"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="13"/>
-      <c r="F15" s="13"/>
-      <c r="G15" s="13"/>
-      <c r="H15" s="13"/>
+      <c r="C15" s="11"/>
+      <c r="D15" s="11"/>
+      <c r="E15" s="11"/>
+      <c r="F15" s="11"/>
+      <c r="G15" s="11"/>
+      <c r="H15" s="11"/>
     </row>
     <row r="16" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="13"/>
-      <c r="D16" s="13"/>
-      <c r="E16" s="13"/>
-      <c r="F16" s="13"/>
-      <c r="G16" s="13"/>
-      <c r="H16" s="13"/>
+      <c r="B16" s="11"/>
+      <c r="C16" s="11"/>
+      <c r="D16" s="11"/>
+      <c r="E16" s="11"/>
+      <c r="F16" s="11"/>
+      <c r="G16" s="11"/>
+      <c r="H16" s="11"/>
     </row>
     <row r="17" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="B17" s="13" t="s">
+      <c r="B17" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="C17" s="13"/>
-      <c r="D17" s="13"/>
-      <c r="E17" s="13"/>
-      <c r="F17" s="13"/>
-      <c r="G17" s="13"/>
-      <c r="H17" s="13"/>
+      <c r="C17" s="11"/>
+      <c r="D17" s="11"/>
+      <c r="E17" s="11"/>
+      <c r="F17" s="11"/>
+      <c r="G17" s="11"/>
+      <c r="H17" s="11"/>
     </row>
     <row r="18" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="B18" s="13" t="s">
+      <c r="B18" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C18" s="13"/>
-      <c r="D18" s="13"/>
-      <c r="E18" s="13"/>
-      <c r="F18" s="13"/>
-      <c r="G18" s="13"/>
-      <c r="H18" s="13"/>
+      <c r="C18" s="11"/>
+      <c r="D18" s="11"/>
+      <c r="E18" s="11"/>
+      <c r="F18" s="11"/>
+      <c r="G18" s="11"/>
+      <c r="H18" s="11"/>
     </row>
     <row r="19" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="13"/>
-      <c r="C19" s="13"/>
-      <c r="D19" s="13"/>
-      <c r="E19" s="13"/>
-      <c r="F19" s="13"/>
-      <c r="G19" s="13"/>
-      <c r="H19" s="13"/>
+      <c r="B19" s="11"/>
+      <c r="C19" s="11"/>
+      <c r="D19" s="11"/>
+      <c r="E19" s="11"/>
+      <c r="F19" s="11"/>
+      <c r="G19" s="11"/>
+      <c r="H19" s="11"/>
     </row>
     <row r="20" spans="1:8" ht="18.75" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="13"/>
-      <c r="C20" s="13"/>
-      <c r="D20" s="13"/>
-      <c r="E20" s="13"/>
-      <c r="F20" s="13"/>
-      <c r="G20" s="13"/>
-      <c r="H20" s="13"/>
+      <c r="B20" s="11"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="11"/>
+      <c r="E20" s="11"/>
+      <c r="F20" s="11"/>
+      <c r="G20" s="11"/>
+      <c r="H20" s="11"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
     <row r="22" spans="1:8" ht="20.25" thickBot="1" x14ac:dyDescent="0.35">
@@ -1303,10 +1298,10 @@
       <c r="A51" s="5" t="s">
         <v>26</v>
       </c>
-      <c r="B51" s="15" t="s">
+      <c r="B51" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C51" s="16"/>
+      <c r="C51" s="14"/>
     </row>
     <row r="52" spans="1:3" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A52" s="4" t="s">
@@ -1319,8 +1314,8 @@
       <c r="A53" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="B53" s="11"/>
-      <c r="C53" s="12"/>
+      <c r="B53" s="15"/>
+      <c r="C53" s="16"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
@@ -1331,8 +1326,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="B13:H13"/>
-    <mergeCell ref="B51:C51"/>
     <mergeCell ref="B52:C52"/>
     <mergeCell ref="B53:C53"/>
     <mergeCell ref="B54:C54"/>
@@ -1349,6 +1342,8 @@
     <mergeCell ref="B16:H16"/>
     <mergeCell ref="B17:H17"/>
     <mergeCell ref="B18:H18"/>
+    <mergeCell ref="B13:H13"/>
+    <mergeCell ref="B51:C51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="76" orientation="portrait" r:id="rId1"/>

</xml_diff>